<commit_message>
Updated template file. Rows now start from row 2. Updated acer return message to be clearer
</commit_message>
<xml_diff>
--- a/Lenovo.xlsx
+++ b/Lenovo.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sziyan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/Development/Python/lenovo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A1C087-48EA-6140-B756-7D0BFE2782C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B600256E-96D8-2D43-8D6A-135976FE56AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{5363B2D6-2EB0-4D25-A03C-29B787119601}"/>
+    <workbookView xWindow="23000" yWindow="2120" windowWidth="29040" windowHeight="15840" xr2:uid="{5363B2D6-2EB0-4D25-A03C-29B787119601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample serial number" sheetId="1" r:id="rId1"/>
+    <sheet name="Models" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,19 +35,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ThinkPad L14</t>
   </si>
   <si>
     <t>PF2L3S40</t>
+  </si>
+  <si>
+    <t>S/N</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Thinkpad E14</t>
+  </si>
+  <si>
+    <t>Thinkpad E490</t>
+  </si>
+  <si>
+    <t>Thinkpad L13</t>
+  </si>
+  <si>
+    <t>Thinkpad L380</t>
+  </si>
+  <si>
+    <t>Thinkpad L390</t>
+  </si>
+  <si>
+    <t>Thinkpad L480</t>
+  </si>
+  <si>
+    <t>Thinkpad X280</t>
+  </si>
+  <si>
+    <t>Thinkpad X390</t>
+  </si>
+  <si>
+    <t>Thinkpad L14</t>
+  </si>
+  <si>
+    <t>Thinkpad X13</t>
+  </si>
+  <si>
+    <t>Thinkbook 13s G2</t>
+  </si>
+  <si>
+    <t>Thinkpad X13 G2</t>
+  </si>
+  <si>
+    <t>Acer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +106,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -71,28 +137,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -430,34 +487,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DD059B-280F-4668-B08C-FCB8E17464E7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A1">
+  <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="1" priority="53"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
+  <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="0" priority="54"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2752DC8D-7EAD-904E-994A-D4C41EB38FDA}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>